<commit_message>
updated the script to create symbol view as well.
There is still a bug, so that the library manager cannot recognize the verilog_rc _*and verilog_rlc_* files... I have posted a question on the cadence forum on how to fix this.
</commit_message>
<xml_diff>
--- a/component_database/component_database.xlsx
+++ b/component_database/component_database.xlsx
@@ -520,7 +520,7 @@
         <v>0.004584090700382463</v>
       </c>
       <c r="E2" t="n">
-        <v>1.807123504968878e-10</v>
+        <v>1.629563790203775e-10</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -549,7 +549,7 @@
         <v>0.01060657049720618</v>
       </c>
       <c r="E3" t="n">
-        <v>2.099852383648819e-10</v>
+        <v>1.917700064493982e-10</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -578,7 +578,7 @@
         <v>0.01988739855929249</v>
       </c>
       <c r="E4" t="n">
-        <v>2.298300616376914e-10</v>
+        <v>2.424361013807798e-10</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -607,7 +607,7 @@
         <v>0.003407941952268195</v>
       </c>
       <c r="E5" t="n">
-        <v>2.466370877003737e-10</v>
+        <v>2.331544095591624e-10</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -636,7 +636,7 @@
         <v>0.005313241259448525</v>
       </c>
       <c r="E6" t="n">
-        <v>3.040911201516682e-10</v>
+        <v>3.075256053032039e-10</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -694,7 +694,7 @@
         <v>0.00288337521837426</v>
       </c>
       <c r="E8" t="n">
-        <v>3.054262897792289e-10</v>
+        <v>3.115217187911944e-10</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -723,7 +723,7 @@
         <v>0.01255450938887008</v>
       </c>
       <c r="E9" t="n">
-        <v>6.965600479637055e-10</v>
+        <v>7.631372149827132e-10</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -752,7 +752,7 @@
         <v>0.01586517434812083</v>
       </c>
       <c r="E10" t="n">
-        <v>4.167555360387524e-10</v>
+        <v>4.463901006559279e-10</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -781,7 +781,7 @@
         <v>0.00695245784763255</v>
       </c>
       <c r="E11" t="n">
-        <v>5.187708761297075e-10</v>
+        <v>5.93988026356113e-10</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -810,7 +810,7 @@
         <v>0.005112436409006512</v>
       </c>
       <c r="E12" t="n">
-        <v>5.42589527900658e-10</v>
+        <v>6.380816707157207e-10</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -839,7 +839,7 @@
         <v>0.002375672633263908</v>
       </c>
       <c r="E13" t="n">
-        <v>3.246890198184251e-10</v>
+        <v>3.542372760906387e-10</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -868,7 +868,7 @@
         <v>0.002738205421581654</v>
       </c>
       <c r="E14" t="n">
-        <v>3.523490910349147e-10</v>
+        <v>3.844681009825206e-10</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -897,7 +897,7 @@
         <v>0.001826270325902945</v>
       </c>
       <c r="E15" t="n">
-        <v>3.405737396374765e-10</v>
+        <v>3.949479671894505e-10</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -926,7 +926,7 @@
         <v>0.009656638436030904</v>
       </c>
       <c r="E16" t="n">
-        <v>5.307604910389628e-10</v>
+        <v>6.78703583943832e-10</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -955,7 +955,7 @@
         <v>0.009656638436030904</v>
       </c>
       <c r="E17" t="n">
-        <v>5.307604910389628e-10</v>
+        <v>6.78703583943832e-10</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -984,7 +984,7 @@
         <v>0.04862458105968567</v>
       </c>
       <c r="E18" t="n">
-        <v>2.700561036155763e-10</v>
+        <v>3.118413771928103e-10</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1089,7 +1089,7 @@
         <v>0.03025119339207952</v>
       </c>
       <c r="E2" t="n">
-        <v>1.179258142825761e-10</v>
+        <v>1.747799862803832e-10</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -1116,7 +1116,7 @@
         <v>0.008664218499631051</v>
       </c>
       <c r="E3" t="n">
-        <v>2.275764406233191e-10</v>
+        <v>2.421235549242754e-10</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>

</xml_diff>